<commit_message>
BERT Embedding extraction finished
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/eda/classification_wo_paraphrase_report.xlsx
+++ b/textToOps/data/processed/eda/classification_wo_paraphrase_report.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.8</v>
       </c>
       <c r="C2" t="n">
         <v>0.8</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8000000000000002</v>
       </c>
       <c r="E2" t="n">
         <v>5</v>
@@ -481,13 +481,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>0.6</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6666666666666665</v>
+        <v>0.7499999999999999</v>
       </c>
       <c r="E3" t="n">
         <v>5</v>
@@ -496,17 +496,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="E4" t="n">
         <v>6</v>
@@ -538,13 +538,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9230769230769231</v>
+        <v>0.8125</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="D6" t="n">
-        <v>0.888888888888889</v>
+        <v>0.8666666666666666</v>
       </c>
       <c r="E6" t="n">
         <v>14</v>
@@ -553,17 +553,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
@@ -579,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
@@ -591,17 +591,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6</v>
+        <v>0.888888888888889</v>
       </c>
       <c r="E9" t="n">
         <v>5</v>
@@ -610,7 +610,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -633,13 +633,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>2</v>
@@ -648,36 +648,36 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7499999999999999</v>
+        <v>0.7692307692307692</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5714285714285715</v>
+        <v>0.5</v>
       </c>
       <c r="E13" t="n">
         <v>2</v>
@@ -686,17 +686,17 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="E14" t="n">
         <v>3</v>
@@ -705,7 +705,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -724,7 +724,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -743,17 +743,17 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
         <v>2</v>
@@ -762,17 +762,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E18" t="n">
         <v>2</v>
@@ -781,17 +781,17 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E19" t="n">
         <v>3</v>
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E20" t="n">
         <v>2</v>
@@ -819,17 +819,17 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8</v>
       </c>
       <c r="E21" t="n">
         <v>2</v>
@@ -838,17 +838,17 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8</v>
       </c>
       <c r="E22" t="n">
         <v>3</v>
@@ -857,17 +857,17 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E23" t="n">
         <v>4</v>
@@ -876,7 +876,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -899,16 +899,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.8390804597701149</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.8390804597701149</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.8390804597701149</v>
       </c>
       <c r="E25" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.8390804597701149</v>
       </c>
     </row>
     <row r="26">
@@ -918,16 +918,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.7171524128045867</v>
+        <v>0.8642080745341615</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7590062111801241</v>
+        <v>0.849792960662526</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7165976535541753</v>
+        <v>0.8361143687230645</v>
       </c>
       <c r="E26" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27">
@@ -937,16 +937,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.7838785245761991</v>
+        <v>0.8644909688013137</v>
       </c>
       <c r="C27" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.8390804597701149</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7719176818014027</v>
+        <v>0.8339040908006425</v>
       </c>
       <c r="E27" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mac backup before paraphrase
</commit_message>
<xml_diff>
--- a/textToOps/data/processed/eda/classification_wo_paraphrase_report.xlsx
+++ b/textToOps/data/processed/eda/classification_wo_paraphrase_report.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8000000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="n">
         <v>5</v>
@@ -477,17 +477,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7499999999999999</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>5</v>
@@ -496,17 +496,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8</v>
+        <v>0.375</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7272727272727272</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="E4" t="n">
         <v>6</v>
@@ -515,17 +515,17 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.7499999999999999</v>
       </c>
       <c r="E5" t="n">
         <v>3</v>
@@ -534,17 +534,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8125</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="C6" t="n">
         <v>0.9285714285714286</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8666666666666666</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E6" t="n">
         <v>14</v>
@@ -553,17 +553,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
@@ -572,7 +572,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -591,17 +591,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D9" t="n">
-        <v>0.888888888888889</v>
+        <v>0.4444444444444445</v>
       </c>
       <c r="E9" t="n">
         <v>5</v>
@@ -610,17 +610,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E10" t="n">
         <v>3</v>
@@ -629,17 +629,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E11" t="n">
         <v>2</v>
@@ -648,17 +648,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.7142857142857143</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7692307692307692</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E12" t="n">
         <v>6</v>
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>2</v>
@@ -686,17 +686,17 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E14" t="n">
         <v>3</v>
@@ -705,17 +705,17 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E15" t="n">
         <v>3</v>
@@ -724,17 +724,17 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E16" t="n">
         <v>4</v>
@@ -743,17 +743,17 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
         <v>2</v>
@@ -762,17 +762,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
         <v>2</v>
@@ -781,17 +781,17 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
         <v>3</v>
@@ -800,17 +800,17 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
         <v>2</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.6666666666666666</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.8</v>
       </c>
       <c r="E21" t="n">
         <v>2</v>
@@ -838,17 +838,17 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8</v>
+        <v>0.7499999999999999</v>
       </c>
       <c r="E22" t="n">
         <v>3</v>
@@ -857,17 +857,17 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
         <v>4</v>
@@ -876,7 +876,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -899,16 +899,16 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.8390804597701149</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8390804597701149</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8390804597701149</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8390804597701149</v>
+        <v>0.6551724137931034</v>
       </c>
     </row>
     <row r="26">
@@ -918,13 +918,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.8642080745341615</v>
+        <v>0.6202380952380953</v>
       </c>
       <c r="C26" t="n">
-        <v>0.849792960662526</v>
+        <v>0.6273291925465838</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8361143687230645</v>
+        <v>0.589095928226363</v>
       </c>
       <c r="E26" t="n">
         <v>87</v>
@@ -937,13 +937,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.8644909688013137</v>
+        <v>0.6685002736726874</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8390804597701149</v>
+        <v>0.6551724137931034</v>
       </c>
       <c r="D27" t="n">
-        <v>0.8339040908006425</v>
+        <v>0.631837255975187</v>
       </c>
       <c r="E27" t="n">
         <v>87</v>

</xml_diff>